<commit_message>
added recusive check to add top stories
</commit_message>
<xml_diff>
--- a/automate_instagram/posts_csv/postedStories.xlsx
+++ b/automate_instagram/posts_csv/postedStories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1471,27 +1471,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>WhateverIWant888</t>
+          <t>KangarooDense</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>“Hey Alexa, what is the distance between the Earth and the Sun?”</t>
+          <t>My uncle just confessed that he had installed a spy camera in my bedroom when I was little.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>“The sun is 94 millio…recalculating…the sun is 93 millio…recalculating…the sun is 84 million mi…recalculating…”</t>
+          <t>It turned out he was the only one who did believe that I wasn't having "imaginary" friends.</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
       <c r="F34" t="n">
-        <v>14236</v>
+        <v>3847</v>
       </c>
       <c r="G34" t="n">
-        <v>1658431146</v>
+        <v>1665834459</v>
       </c>
     </row>
     <row r="35">
@@ -1502,27 +1502,1296 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>trexwins</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>My daughter smiled at the mother rabbit and her babies.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>She cried at what the mother did after I sneezed.</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1652</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1667232657</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>tinyarmtrex88</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>“It’s okay, darling, the new babysitter is here to put you to bed,” my mother said as she hugged me and smiled at the young woman behind her.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>I’m surprised she couldn’t feel me shaking as I looked upon the face that I’d been seeing outside my window for weeks.</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F36" t="n">
+        <v>20019</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1591817346</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Keeenwaaa</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>My father seemed distressed even though it looked like he'd bought so many new gold trinkets.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>As I snuck up to him and gave him a hug, he dropped the gold food in his hand and looked at me with horror.</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F37" t="n">
+        <v>11912</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1639723251</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>[deleted]</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>I shined my flashlight over the cabinet of porcelin dolls.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Their pupils contracted.</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F38" t="n">
+        <v>17518</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1595944680</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Jakeh7494</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>It was my first time with an uncircumcised man, but I had watched a few videos on what to do, so I got down on both knees, ready to rock his world.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>As I peeled back his foreskin, nothing could’ve prepared me for the hundreds of spiders that scurried out from underneath.</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4477</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1667246277</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>sugar-soad</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>My younger sister lay on the couch weeping as her partner desperately tried to comfort her</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>I felt terrible about slipping her the abortion pills, but my wedding is in a few months and I don't want her to be the center of attention</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F40" t="n">
+        <v>14726</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1644488940</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Arkady2009</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>[JAN22] My (42F) daughter (13F) took her own life last week after being subjected to online trolling, and today the police arrested ME!</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>The emails I sent pretending to be her school crush were to try and toughen her up - she’s always been a cry baby and her suicide was just another attempt at attention.</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F41" t="n">
+        <v>12502</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1643538230</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Tired_Autistic</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Today an alien ship landed on Earth, however there's one tiny problem.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>It's empty.</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4505</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1666335244</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>meowmancer2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>As the noose took away my last breath I thought happily my life of crippling debt was finally over.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>I awoke in the hospital to discover I would now owe a further million in medical costs for saving my life.</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2361</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1666553645</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>normancrane</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Despite our children's sobbing protest, after our beloved dog gave birth to puppies we ultimately decided to drown them.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>The puppies just seemed easier to care for.</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4128</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1666398545</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>[deleted]</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Trapped and starving in a World War I trench, I gave my last ration to my best friend and partner.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Adolf seems so passionate about having a future in politics, it would be wrong to let him die.</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F45" t="n">
+        <v>20363</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1589849137</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SilverSeregios</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>"In sorry, but there's nothing we can do," the doctor said to me while he turned off the machine.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>As my lungs began to fail, and vision go dark, the doctor left and added, "There's just been a shortage of organ donors."</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F46" t="n">
+        <v>11911</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1640449227</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TipsSlight</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>I promised my wife that when I return from the war, we'd sit down and rewatch the movie from our first date.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>But now she's dying in the hospital, all because she wanted to make popcorn.</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F47" t="n">
+        <v>21944</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1583372308</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TortCourt</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>All my life, I wished Pokémon were real, so I was ecstatic when my wish came true last week.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>But when reports started flooding in of massive earthquakes, summer ice storms, and children disappearing from their own birthday parties, I realized that having only 300 people in each game wasn't due to constraints on Game Boy technology.</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F48" t="n">
+        <v>12920</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1660058812</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Ezra_Pound_</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>The genie told me I could have dinner with any five people from history, living or dead, so I chose Abraham Lincoln, John Dillinger, the Zodiac Killer, Marilyn Monroe, and my dear departed grandfather.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>“I said you could choose five people,” he said.</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F49" t="n">
+        <v>14590</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1644662522</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>KangarooDense</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Back when I was an exorcist, a little girl came up to me with bruises all over her body and told me her father was possessed.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>"I think the demon was in here," she said with innocent eyes, holding up what looked like an empty liquor bottle.</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F50" t="n">
+        <v>13524</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1657109315</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Melonwolfii</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>As I was shown the statistics of my life after death, I stared in horror at the 27 'assist kills.'</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>The horror was far more striking for me, seeing as I was a suicide hotline worker.</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F51" t="n">
+        <v>14034</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1642436061</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Sisyphuzz</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>When we set out for our camping trip I told my son “NEVER answer voices calling your name in the woods…”</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Three days after getting separated, our search party still hasn’t found him.</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2085</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1666033501</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TylerSpicknell</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>I had finally beaten the final boss on the game, which was something that no one had ever done before!</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>It told me "Thank you for freeing my spirit, but now you will take my place until someone beats you as well!"</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F53" t="n">
+        <v>5906</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1645458097</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>KangarooDense</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>"I'm so sorry, dad, but please don't come near me!" was the last thing my son said before blowing his head off.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>As the bitemark on his arm began to heal, I wished I had told him sooner that our family was immune.</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F54" t="n">
+        <v>11696</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1645280659</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Blakman07</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>As a soldier I’ve seen a lot of death and men cry out for their moms as they die. But it was weird hearing that guy yesterday call out to his father as we nailed him to the cross.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F55" t="n">
+        <v>7865</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1661985834</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>iceariina</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>"I'll be your server," she said as she placed a menu before me on the table.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>My blood ran cold when she smiled at the empty seat across from me, set down a kids' menu, and walked away.</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F56" t="n">
+        <v>5426</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1661720771</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Zjoriek</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Here I am: trying my best to swim while slowly bleeding to death as I see the boat sailing away.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>"What do they even need my fins for?"</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="F57" t="n">
+        <v>22663</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1582629209</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TheRealWingnut</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>I had trained for this for years and I rejoiced as I lifted the barbell over my head, finally beat the world record for the bench press.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Time seemed to slow to a crawl, however, as I felt both of my wrists break and the barbell descended toward my neck</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F58" t="n">
+        <v>7080</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1665227988</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>EarthMarsUranus</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>It's been almost a decade since I last saw my mother.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>And she still reminds me every day that if I misbehave again she'll take my hearing too.</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F59" t="n">
+        <v>25120</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1574862605</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>EldritchEggoWaffle</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>My dog suddenly walked over to me and began staring at me with a very odd look in his eyes.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Without warning, he opened his mouth and said: "We need to talk and we don't have much time before He gets here."</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F60" t="n">
+        <v>7253</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1645913546</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JinxXedOmens</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>A prophet from above came down to earth and revealed to humanity the truth behind what comes after death.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>That was two months ago, and at the last global census they counted an estimated 200,000 humans remain.</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F61" t="n">
+        <v>5516</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1656373028</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>bee875</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>When the witch told me I would die on a Friday, I took it to my advantage doing dangerous things every other day knowing I wouldn't die.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Little did I know that it would take 2 days for my body to finally give out in the collapsed glacier cave, lost and alone.</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F62" t="n">
+        <v>10209</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1645067318</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ShakespearesNutSack</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>I'm finally leaving my abusive husband.</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>I smile, hold my son tight, and we board the unsinkable ship.</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F63" t="n">
+        <v>8193</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1656291094</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ntgco</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>The zombie horde was easy to survive; mother nature took the vast majority through natural decomposition.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>We've been hiding for decades from the hurricane of biting flies that consume everything dead....or alive.</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F64" t="n">
+        <v>5943</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1663246676</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>WrenchLover</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>I've been a firefighter for 25 years, and I have four beautiful young children.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>My heart began to beat faster as our fire truck turned toward my house.</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F65" t="n">
+        <v>4832</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1642662697</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>demhammmys</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>As the poppers blew the color blue at the gender reveal party.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>The relief was my only hope he wouldn’t do to a little boy what he does to me.</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F66" t="n">
+        <v>7966</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1640352795</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Vesurel</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Today is the last day you'll be human.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>And the first day you'll be yourself.</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F67" t="n">
+        <v>6791</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1651565565</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>JokerCrowe</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>"It seems you have discovered an entirely new type of termite".</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>I felt the terror rise in my chest as the doctor turned around with the x-rays; "this also explains the 'aching' you've been feeling in your bones".</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F68" t="n">
+        <v>21302</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1594998216</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>sunnyflouwer</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>I always put €5 under my child's pillow when he loses a milk tooth.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+There have been 65 teeth under his pillow so far and I am running out of money for this month.</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F69" t="n">
+        <v>8156</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1657709362</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>UncomfyUnicorn</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>I remember how Albert Einstein once basically said that after nuclear war we all end up back at the Stone Age.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>But as we kept excavating the ancient power plant, we began to understand it had happened many times already.</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F70" t="n">
+        <v>3583</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1667849583</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DegenerateGeometry</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>The math professor felt in his bones that tonight was the night that he'd finally prove the deepeat mystery in all mathematics: the Riemann Hypothesis.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>The next morning his colleagues found his body, slumped forward in his chair, having clawed and gouged his eyes out.</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F71" t="n">
+        <v>895</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1668209193</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Sir_Oragon</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>The year is 20632, and humanity has just made what could be the largest scientific discovery ever.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>One of our oldest satellites cannot travel any further; we have found the edge of the universe.
+Edit: guys, my math isn't infallible; I'm more scared of my exams than the end of the universe. And I meant a probe, not a satellite. Apologies for the confusion!</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="F72" t="n">
+        <v>14275</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1643894402</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
           <t>Dakingtrex</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>"So tell me sir, can your device really tell the shape shifters apart from humanity?"</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>"No, it's but another one of my failed inventions, sadly," I lied, hoping he didn't see the sweat upon my brow as I shakily reached for my gun.</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="E73" t="n">
         <v>0.99</v>
       </c>
-      <c r="F35" t="n">
-        <v>16309</v>
-      </c>
-      <c r="G35" t="n">
+      <c r="F73" t="n">
+        <v>16315</v>
+      </c>
+      <c r="G73" t="n">
         <v>1637557558</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Nordinaren346</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>"I never name my livestock, makes killing and eating them that much harder!"</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>His words echoed in my mind as I had become hung up on the fact that not once during our interrogation had he referred to his missing children by name.</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F74" t="n">
+        <v>5414</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1653676319</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>JamesTIA</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Timmy and I were playing with his toy phone when I suggested he use it to call up his imaginary friend.</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>In a horrifying moment of clarity, I could feel my cell phone vibrating in my pocket.</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F75" t="n">
+        <v>12591</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1646966787</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>TwoSentenceHorror</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>the_martell_kidd</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>They say what doesn’t kill you makes you stronger.</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>But I really think I should’ve listened to those cave dive warnings.</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="F76" t="n">
+        <v>5393</v>
+      </c>
+      <c r="G76" t="n">
+        <v>1657210705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>